<commit_message>
basic main ui dev
</commit_message>
<xml_diff>
--- a/devSchedule.xlsx
+++ b/devSchedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Silly\Homework\2dGamePrograming\lastProject\2DGPLastProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CBD3FA-F3E8-4D99-960E-A7A5F28D6015}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E18E03-B171-4D54-9753-AB5A8A766BFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B1245899-F770-42B1-8C32-F60881BD91D9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>1주차</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,9 +78,6 @@
   <si>
     <t>변경점</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">적 </t>
   </si>
   <si>
     <t>아군</t>
@@ -215,10 +212,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>적 화면에 출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>적 리소스 수집</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -232,6 +225,25 @@
   </si>
   <si>
     <t>맵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.spriters-resource.com/playstation/shinmegamitensei/</t>
+  </si>
+  <si>
+    <t>적, 조작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>적 화면에 출력, 인터페이스 조작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문자에 대한 표시 방법을 배우지 못하여 구현 실패</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 메뉴만 구성, 나머지는 조작을 배운 뒤 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -656,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A13F27-D58D-46A6-9749-9B628960E2FF}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -667,10 +679,11 @@
     <col min="1" max="1" width="12.75" customWidth="1"/>
     <col min="2" max="2" width="27.125" customWidth="1"/>
     <col min="3" max="3" width="50.375" customWidth="1"/>
-    <col min="4" max="4" width="42.375" customWidth="1"/>
+    <col min="4" max="4" width="44.375" customWidth="1"/>
+    <col min="5" max="5" width="57" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -684,155 +697,162 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -847,10 +867,10 @@
         <v>8</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="3"/>
     </row>
@@ -865,10 +885,10 @@
         <v>9</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="3"/>
     </row>
@@ -935,26 +955,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
game_world and enemy Bd bar
</commit_message>
<xml_diff>
--- a/devSchedule.xlsx
+++ b/devSchedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Silly\Homework\2dGamePrograming\lastProject\2DGPLastProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71F3CCB-1D13-4C99-B039-4B51856585EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D11AFA-22FC-4109-A36D-4C30444D3ED9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B1245899-F770-42B1-8C32-F60881BD91D9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>1주차</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -256,6 +256,14 @@
   </si>
   <si>
     <t>다시 메인 메뉴 구성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아군과 적군의 class 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스킬 ui 등 각종 제작</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -683,7 +691,7 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -792,7 +800,9 @@
       <c r="C8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
@@ -800,7 +810,9 @@
       <c r="C9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
@@ -973,6 +985,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
@@ -983,16 +1005,6 @@
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>